<commit_message>
mas inserts y correcciones en triggers ahora que hay datos para probar
</commit_message>
<xml_diff>
--- a/Creaciones/Carga_de_datos_TP_Activas_Concatenar.xlsx
+++ b/Creaciones/Carga_de_datos_TP_Activas_Concatenar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Facultad\CUARTO AÑO\Base de datos avanzadas\Trabajo Practico\TP_DBA\Creaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7338B429-BD26-41F9-A5E1-9687838C84A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE13E874-6BB4-4DC5-B421-6EB358A9E08E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="12" xr2:uid="{07F8E7B2-9205-4136-B2D9-1DF552422D8E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="13" activeTab="16" xr2:uid="{07F8E7B2-9205-4136-B2D9-1DF552422D8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Loacalizaciones" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="146">
   <si>
     <t>provincia</t>
   </si>
@@ -232,15 +232,6 @@
     <t>id_finalidad</t>
   </si>
   <si>
-    <t>sdf</t>
-  </si>
-  <si>
-    <t>contrato_estados</t>
-  </si>
-  <si>
-    <t>sdfsdf</t>
-  </si>
-  <si>
     <t>ContratoAlquiler</t>
   </si>
   <si>
@@ -461,6 +452,36 @@
   </si>
   <si>
     <t>Juan Ignacio Gerstner</t>
+  </si>
+  <si>
+    <t>Vacaciones</t>
+  </si>
+  <si>
+    <t>Ocupacion temporal</t>
+  </si>
+  <si>
+    <t>Negocios</t>
+  </si>
+  <si>
+    <t>otros</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
+  </si>
+  <si>
+    <t>Baja a pedido del cliente</t>
+  </si>
+  <si>
+    <t>Baja a pedido del dueño</t>
+  </si>
+  <si>
+    <t>contratos_estados</t>
+  </si>
+  <si>
+    <t>10-05-2021</t>
   </si>
 </sst>
 </file>
@@ -502,10 +523,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -900,7 +922,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -912,7 +934,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -924,7 +946,7 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -936,7 +958,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -996,13 +1018,13 @@
         <v>41154249</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G3">
         <f>Direcciones!B3</f>
@@ -1021,13 +1043,13 @@
         <v>39717392</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G4">
         <f>Direcciones!B4</f>
@@ -1046,13 +1068,13 @@
         <v>42560204</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G5">
         <f>Direcciones!B5</f>
@@ -1243,7 +1265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F55617-8BD6-476E-B9EE-BF5B22784FA6}">
   <dimension ref="A2:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
@@ -1434,7 +1456,7 @@
   <dimension ref="A2:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,16 +1546,17 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C90E7A4-180C-4E0D-93BF-9A42355C5974}">
-  <dimension ref="A2:C3"/>
+  <dimension ref="A2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="82.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1550,13 +1573,49 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("insert into"," ",$A$2, "(",$B$2,", ",$C$2,") values (", B3,", '",C3,"');")</f>
-        <v>insert into contratos_finalidades(id_finalidad, descripcion) values (2, 'sdf');</v>
+        <v>insert into contratos_finalidades(id_finalidad, descripcion) values (1, 'Vacaciones');</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A6" si="0">CONCATENATE("insert into"," ",$A$2, "(",$B$2,", ",$C$2,") values (", B4,", '",C4,"');")</f>
+        <v>insert into contratos_finalidades(id_finalidad, descripcion) values (2, 'Ocupacion temporal');</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into contratos_finalidades(id_finalidad, descripcion) values (3, 'Negocios');</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into contratos_finalidades(id_finalidad, descripcion) values (4, 'otros');</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1566,20 +1625,21 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD6900A-28DB-4B8D-BFE3-A23147DD58A8}">
-  <dimension ref="A2:C3"/>
+  <dimension ref="A2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="69.28515625" customWidth="1"/>
+    <col min="1" max="1" width="80.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
@@ -1591,13 +1651,49 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("insert into"," ",$A$2, "(",$B$2,", ",$C$2,") values (", B3,", '",C3,"');")</f>
-        <v>insert into contrato_estados(id_estado, descripcion) values (213, 'sdfsdf');</v>
+        <v>insert into contratos_estados(id_estado, descripcion) values (1, 'Activo');</v>
       </c>
       <c r="B3">
-        <v>213</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A6" si="0">CONCATENATE("insert into"," ",$A$2, "(",$B$2,", ",$C$2,") values (", B4,", '",C4,"');")</f>
+        <v>insert into contratos_estados(id_estado, descripcion) values (2, 'Finalizado');</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into contratos_estados(id_estado, descripcion) values (3, 'Baja a pedido del cliente');</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into contratos_estados(id_estado, descripcion) values (4, 'Baja a pedido del dueño');</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1609,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAA835C-F8A9-4D3F-8437-36FDBA866345}">
   <dimension ref="A2:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,7 +1719,7 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>49</v>
@@ -1632,56 +1728,54 @@
         <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="I2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("insert into"," ",$A$2, "(",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,", ",$H$2,", ",$I$2,") values (", B3,", ",C3,", '",D3,"', ",E3,", ",F3,", ",G3,", ",H3,", ",I3,");")</f>
-        <v>insert into ContratoAlquiler(id_inmueble, id_cliente, fechacontrato, id_estado, periodo_vigencia, vencimiento_cuota, id_finalidad, precio_inicial) values (1, 1, 'text', 213, 4444, 4444, 2, 4444);</v>
+        <v>insert into ContratoAlquiler(id_inmueble, id_cliente, fechacontrato, id_estado, periodo_vigencia, vencimiento_cuota, id_finalidad, precio_inicial) values (1000, 1, '10-05-2021', 1, 6, 44510, 2, 1500);</v>
       </c>
       <c r="B3">
-        <f>Inmueble!B3</f>
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="C3">
         <f>Clientes!B3</f>
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
       <c r="E3">
         <f>contrato_estados!B3</f>
-        <v>213</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>4444</v>
-      </c>
-      <c r="G3">
-        <v>4444</v>
+        <v>6</v>
+      </c>
+      <c r="G3" s="3">
+        <v>44510</v>
       </c>
       <c r="H3">
-        <f>contratos_finalidades!B3</f>
         <v>2</v>
       </c>
       <c r="I3">
-        <v>4444</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1746,10 +1840,10 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -1811,13 +1905,13 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>45</v>
@@ -1829,7 +1923,7 @@
         <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1959,7 +2053,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D3">
         <v>3100</v>
@@ -2016,7 +2110,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D6">
         <v>5800</v>
@@ -2034,7 +2128,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D7">
         <v>3000</v>
@@ -2052,7 +2146,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D8">
         <v>3000</v>
@@ -2070,7 +2164,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D9">
         <v>3100</v>
@@ -2137,7 +2231,7 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>49</v>
@@ -2146,10 +2240,10 @@
         <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2168,7 +2262,7 @@
         <v>123</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2275,19 +2369,19 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E3">
         <v>1276</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2302,19 +2396,19 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E4">
         <v>2052</v>
       </c>
       <c r="F4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2329,19 +2423,19 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E5">
         <v>111</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2410,19 +2504,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F3">
         <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2434,19 +2528,19 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F4">
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2458,19 +2552,19 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2482,19 +2576,19 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2538,10 +2632,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2553,10 +2647,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2568,10 +2662,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2583,10 +2677,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2705,7 +2799,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -2723,7 +2817,7 @@
         <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2735,7 +2829,7 @@
         <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2747,7 +2841,7 @@
         <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2759,7 +2853,7 @@
         <v>104</v>
       </c>
       <c r="C6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2771,7 +2865,7 @@
         <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2783,7 +2877,7 @@
         <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2825,7 +2919,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2837,7 +2931,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2872,7 +2966,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
@@ -2890,7 +2984,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2902,7 +2996,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2914,7 +3008,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2926,7 +3020,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se pusieron otros inserts, se corrigieron trigger y vistas
</commit_message>
<xml_diff>
--- a/Creaciones/Carga_de_datos_TP_Activas_Concatenar.xlsx
+++ b/Creaciones/Carga_de_datos_TP_Activas_Concatenar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Facultad\CUARTO AÑO\Base de datos avanzadas\Trabajo Practico\TP_DBA\Creaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE13E874-6BB4-4DC5-B421-6EB358A9E08E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEB96FB-D54E-4C59-8538-79B4BAD2799B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="13" activeTab="16" xr2:uid="{07F8E7B2-9205-4136-B2D9-1DF552422D8E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="14" activeTab="18" xr2:uid="{07F8E7B2-9205-4136-B2D9-1DF552422D8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Loacalizaciones" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="150">
   <si>
     <t>provincia</t>
   </si>
@@ -121,9 +121,6 @@
     <t>tipo_vigencia</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
     <t>Divisas</t>
   </si>
   <si>
@@ -482,6 +479,21 @@
   </si>
   <si>
     <t>10-05-2021</t>
+  </si>
+  <si>
+    <t>Recibo de Sueldo</t>
+  </si>
+  <si>
+    <t>Titulo de propiedad</t>
+  </si>
+  <si>
+    <t>Daniel XL</t>
+  </si>
+  <si>
+    <t>El Cejas</t>
+  </si>
+  <si>
+    <t>Jaun del Gualeyan</t>
   </si>
 </sst>
 </file>
@@ -859,7 +871,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -922,7 +934,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -934,7 +946,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -946,7 +958,7 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -958,7 +970,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -985,22 +997,22 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" t="s">
         <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
@@ -1018,13 +1030,13 @@
         <v>41154249</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" t="s">
         <v>128</v>
-      </c>
-      <c r="F3" t="s">
-        <v>129</v>
       </c>
       <c r="G3">
         <f>Direcciones!B3</f>
@@ -1043,13 +1055,13 @@
         <v>39717392</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" t="s">
         <v>131</v>
-      </c>
-      <c r="F4" t="s">
-        <v>132</v>
       </c>
       <c r="G4">
         <f>Direcciones!B4</f>
@@ -1068,13 +1080,13 @@
         <v>42560204</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" t="s">
         <v>134</v>
-      </c>
-      <c r="F5" t="s">
-        <v>135</v>
       </c>
       <c r="G5">
         <f>Direcciones!B5</f>
@@ -1114,13 +1126,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1195,13 +1207,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1279,19 +1291,19 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
@@ -1300,10 +1312,10 @@
         <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1469,22 +1481,22 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" t="s">
         <v>55</v>
-      </c>
-      <c r="F2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1500,13 +1512,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1561,13 +1573,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
         <v>60</v>
       </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1579,7 +1591,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1591,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1603,7 +1615,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1615,7 +1627,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1639,13 +1651,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1657,7 +1669,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1669,7 +1681,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1681,7 +1693,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1693,7 +1705,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAA835C-F8A9-4D3F-8437-36FDBA866345}">
   <dimension ref="A2:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1719,31 +1731,31 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
         <v>64</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1759,7 +1771,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E3">
         <f>contrato_estados!B3</f>
@@ -1830,41 +1842,48 @@
   <dimension ref="A2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A6"/>
+      <selection activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.5703125" customWidth="1"/>
+    <col min="1" max="1" width="73.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("insert into"," ",$A$2, "(",$B$2,", ",$C$2,") values (", B3,", '",C3,"');")</f>
-        <v>insert into TipoGarantia(id_garantia, descripcion) values (44, 'text');</v>
+        <v>insert into TipoGarantia(id_garantia, descripcion) values (1, 'Recibo de Sueldo');</v>
       </c>
       <c r="B3">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" ref="A4:A6" si="0">CONCATENATE("insert into"," ",$A$2, "(",$B$2,", ",$C$2,") values (", B4,", '",C4,"');")</f>
-        <v>insert into TipoGarantia(id_garantia, descripcion) values (, '');</v>
+        <v>insert into TipoGarantia(id_garantia, descripcion) values (2, 'Titulo de propiedad');</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1888,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B55EA13-CEC4-44B7-84F7-34CD6AA8981C}">
   <dimension ref="A2:G6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,76 +1924,85 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("insert into"," ",$A$2, "(",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,") values ('", B3,"', ",C3,", ",D3,", '",E3,"', '",F3,"', ",G3,");")</f>
-        <v>insert into Garante(dni, id_inmuble, id_cliente, nombre, fechanacimiento, id_tipogarantia) values ('555', 1, 1, 'text', 'text', 44);</v>
+        <v>insert into Garante(dni, id_inmuble, id_cliente, nombre, fechanacimiento, id_tipogarantia) values ('25828924', 1000, 1, 'Daniel XL', '35176', 1);</v>
       </c>
       <c r="B3">
-        <v>555</v>
+        <v>25828924</v>
       </c>
       <c r="C3">
-        <f>Inmueble!B3</f>
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D3">
         <f>Clientes!B3</f>
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
+        <v>147</v>
+      </c>
+      <c r="F3" s="3">
+        <v>35176</v>
       </c>
       <c r="G3">
         <f>TipoGarantia!B3</f>
-        <v>44</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" ref="A4:A6" si="0">CONCATENATE("insert into"," ",$A$2, "(",$B$2,", ",$C$2,", ",$D$2,", ",$E$2,", ",$F$2,", ",$G$2,") values ('", B4,"', ",C4,", ",D4,", '",E4,"', '",F4,"', ",G4,");")</f>
-        <v>insert into Garante(dni, id_inmuble, id_cliente, nombre, fechanacimiento, id_tipogarantia) values ('', 2, 2, '', '', 0);</v>
+        <v>insert into Garante(dni, id_inmuble, id_cliente, nombre, fechanacimiento, id_tipogarantia) values ('41154249', 1002, 3, 'El Cejas', '36691', 2);</v>
+      </c>
+      <c r="B4">
+        <v>41154249</v>
       </c>
       <c r="C4">
-        <f>Inmueble!B4</f>
-        <v>2</v>
+        <v>1002</v>
       </c>
       <c r="D4">
-        <f>Clientes!B4</f>
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F4" s="3">
+        <v>36691</v>
       </c>
       <c r="G4">
         <f>TipoGarantia!B4</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>insert into Garante(dni, id_inmuble, id_cliente, nombre, fechanacimiento, id_tipogarantia) values ('', 3, 3, '', '', 0);</v>
+        <v>insert into Garante(dni, id_inmuble, id_cliente, nombre, fechanacimiento, id_tipogarantia) values ('11111111', 3, 3, 'Jaun del Gualeyan', '37077', 1);</v>
+      </c>
+      <c r="B5">
+        <v>11111111</v>
       </c>
       <c r="C5">
         <f>Inmueble!B5</f>
@@ -1984,9 +2012,14 @@
         <f>Clientes!B5</f>
         <v>3</v>
       </c>
+      <c r="E5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="3">
+        <v>37077</v>
+      </c>
       <c r="G5">
-        <f>TipoGarantia!B5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2053,7 +2086,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3">
         <v>3100</v>
@@ -2110,7 +2143,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6">
         <v>5800</v>
@@ -2128,7 +2161,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7">
         <v>3000</v>
@@ -2146,7 +2179,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D8">
         <v>3000</v>
@@ -2164,7 +2197,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9">
         <v>3100</v>
@@ -2231,19 +2264,19 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2262,7 +2295,7 @@
         <v>123</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2369,19 +2402,19 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E3">
         <v>1276</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2396,19 +2429,19 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4">
         <v>2052</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2423,19 +2456,19 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5">
         <v>111</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2504,19 +2537,19 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
         <v>93</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="F3">
         <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2528,19 +2561,19 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F4">
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2552,19 +2585,19 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" t="s">
         <v>102</v>
       </c>
-      <c r="D5" t="s">
-        <v>103</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2576,19 +2609,19 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s">
         <v>104</v>
       </c>
-      <c r="D6" t="s">
-        <v>105</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2611,16 +2644,16 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>28</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2632,10 +2665,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" t="s">
         <v>106</v>
-      </c>
-      <c r="D3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2647,10 +2680,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" t="s">
         <v>108</v>
-      </c>
-      <c r="D4" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2662,10 +2695,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
         <v>110</v>
-      </c>
-      <c r="D5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2677,10 +2710,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2704,16 +2737,16 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>31</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2799,13 +2832,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2817,7 +2850,7 @@
         <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2829,7 +2862,7 @@
         <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2841,7 +2874,7 @@
         <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2853,7 +2886,7 @@
         <v>104</v>
       </c>
       <c r="C6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2865,7 +2898,7 @@
         <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2877,7 +2910,7 @@
         <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2901,13 +2934,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2919,7 +2952,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2931,7 +2964,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2966,13 +2999,13 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2984,7 +3017,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2996,7 +3029,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3008,7 +3041,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3020,7 +3053,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>